<commit_message>
first page scrapping done
</commit_message>
<xml_diff>
--- a/euka_brands_data.xlsx
+++ b/euka_brands_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>
@@ -659,447 +659,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>theviraltiktokshopdeals</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>theviraltiktokshopdeals</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>25 days ago</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>itsmarvymarv</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>itsmarvymarv</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>a month ago</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>amandaupnext</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>amandaupnext</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>a month ago</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>heidiann__</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>heidiann__</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>a month ago</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>savannahraeeeeeee</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>savannahraeeeeeee</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>13 days ago</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>lindseyhoughh</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>lindseyhoughh</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>25 days ago</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>jasminemonique_22</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>jasminemonique_22</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>16 days ago</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>humble_beginnings26</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>humble_beginnings26</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>a month ago</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>mikaylanogueira</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>mikaylanogueira</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>13 days ago</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ari1.vv</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>ari1.vv</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>20 days ago</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Beachwaver B1 - Midnight Rose</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>$99.00</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>$35.5M</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Wavytalk Blowout Boost Ionic Thermal Brush 1 1/2 Inch with LED Display, 300℉-420℉ for Different Hair Types, 120-240V Universal Voltage</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>$37.41</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>$31.2M</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>GuruNanda Cocomint Pulling Oil with 7 Essential Oils &amp; Vitamins D, E &amp; K2 - 8 oz</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>$14.99</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>$28.3M</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>(NEW) BODY GLAZE: Pick your favorite scent!</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>$25.00</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>$26.9M</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>The Balance Bundle - Feminine Hygiene Self Care Products</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>$224.00</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>$24.6M</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>LIP LINER STAY-N - Peel-Off Lip Liner Stain - All Day &amp; Night Lipliner with Hyaluronic Acid &amp; Vitamin E - Long Lasting Formula - 0.12 fl oz / 3.5 ml</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>$14.00</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>$23.3M</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>GOPURE Neck Cream Tighten &amp; Lift Firming Cream for Crepey Skin</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>$39.00</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>$21.2M</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>EVIL GOODS! Whipped Beef Tallow &amp; Manuka Honey Organic Nourishing Face Cream Moisturizer Body Lotion Skin Care Lip Balm Hydrating Moisturizing 100% Natural Ingredients - Oil</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>$69.99</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>$18.3M</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>TikTok Exclusive - MySmile Original Dental Grade Teeth Whitening Kit w/ 2 Free Wipes, 5x LED Light, 3 of 18% Carbamide Peroxide Gels, 10-Min Fast Whitening, Non-Sensitive Formula, Removes Coffee/Wine/Smoke Stains</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>$55.99</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>$16.3M</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>[medicube] Affordable Glass Glow Skincare Set | Includes 8 TOP-SELLING products for Gentle Skin Renewal</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>$93.00</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>$14.9M</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>2025-08-29 11:25:26</t>
+          <t>2025-08-29 11:33:48</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
page 2 scrapped succesfully
</commit_message>
<xml_diff>
--- a/euka_brands_data.xlsx
+++ b/euka_brands_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,227 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-08-29 11:33:48</t>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MySmileUS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$37,978,600</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>American Seair Imports</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>825</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$31,078,100</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>simplymandys</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$29,121,000</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mighty Life</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$25,788,900</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cocomint Beauty</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$25,745,000</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>OQ HAIR SHOP</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$25,718,500</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>SACHEU Beauty</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$25,248,400</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>The Ordinary</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>172</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$24,756,600</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ONE SIZE BEAUTY</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$23,656,500</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Color Wow Hair</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$22,923,600</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-08-29 11:40:39</t>
         </is>
       </c>
     </row>

</xml_diff>